<commit_message>
Updated the Master Table with ECLSS and a few other things
</commit_message>
<xml_diff>
--- a/MSDO/MasterTable_rev1.xlsx
+++ b/MSDO/MasterTable_rev1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="812" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" tabRatio="812" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="MasterList" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="Surface Habitat" sheetId="19" r:id="rId16"/>
     <sheet name="ECLSS" sheetId="20" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="413">
   <si>
     <t>Modules</t>
   </si>
@@ -1059,6 +1059,216 @@
   </si>
   <si>
     <t>calls multiple functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat_Volume </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat_Mass </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crew_Activity.EVA_Freq </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crew_Activity.CM_EVA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crew_Activity.EVA_Dur </t>
+  </si>
+  <si>
+    <t>events/week</t>
+  </si>
+  <si>
+    <t>ppl/event</t>
+  </si>
+  <si>
+    <t>hours/person</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARS_2040.Surface_Duration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabin_Pressure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas_Constant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2_Mol_Ratio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_Mol_Ratio </t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat_Leakage_Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat_CO2_Generation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat_O2_Consumption </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPA_Efficiency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WPA_Efficiency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth_Food_Mass </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth_Food_Volume </t>
+  </si>
+  <si>
+    <t>percentage of food to be grown on Mars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrewTime_FoodGrowth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mars_Food_Prep </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth_Food_Prep </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Oxygen_Loss_Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Airlock_Volume </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Airlock_Gas_Loss </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Oxygen_Consumption </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_CO2_Production </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Cooling_Loss </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVA_Water_Consumption </t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>engineering decision</t>
+  </si>
+  <si>
+    <t>J/K*mol</t>
+  </si>
+  <si>
+    <t>BVAD pg. 28</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>%/day</t>
+  </si>
+  <si>
+    <t>kg/CM/day</t>
+  </si>
+  <si>
+    <t>BVAD pg. 50</t>
+  </si>
+  <si>
+    <t>efficiency to reuse water from urine flush</t>
+  </si>
+  <si>
+    <t>efficiency to reuse waste water</t>
+  </si>
+  <si>
+    <t>BVAD pg. 56</t>
+  </si>
+  <si>
+    <t>CM*hr/m^3/yr</t>
+  </si>
+  <si>
+    <t>BVAD pg. 163</t>
+  </si>
+  <si>
+    <t>CM*hr/CM*day</t>
+  </si>
+  <si>
+    <t>BVAD pg. 109</t>
+  </si>
+  <si>
+    <t>time to prepare food grown on Mars</t>
+  </si>
+  <si>
+    <t>time to prepare food brought from earth</t>
+  </si>
+  <si>
+    <t>kg/CM/hr</t>
+  </si>
+  <si>
+    <t>BVAD 131</t>
+  </si>
+  <si>
+    <t>BVAD pg 139</t>
+  </si>
+  <si>
+    <t>BVAD pg 131</t>
+  </si>
+  <si>
+    <t>MarsOne</t>
+  </si>
+  <si>
+    <t>BVAD pg. 139</t>
+  </si>
+  <si>
+    <t>BVAD pg. 130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results.ECLSS.Consumables_Mass </t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Consumables_Volume</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Spares_Mass</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Spares_Volume</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Mass</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Power</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Volume</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Replacements_Mass</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Replacements_Volume</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Lighting_Mass</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Lighting_Volume</t>
+  </si>
+  <si>
+    <t>Results.ECLSS.Lighting_Power</t>
   </si>
 </sst>
 </file>
@@ -1082,21 +1292,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1124,13 +1336,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1194,7 +1406,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1229,7 +1441,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1758,11 +1970,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,13 +2094,22 @@
         <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>192</v>
+      </c>
+      <c r="F7">
+        <v>1250</v>
       </c>
       <c r="G7" t="s">
-        <v>189</v>
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>193</v>
       </c>
       <c r="J7" t="s">
-        <v>209</v>
+        <v>190</v>
+      </c>
+      <c r="K7" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -1896,22 +2117,19 @@
         <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F8">
-        <v>1250</v>
+        <v>6.7799999999999996E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>195</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J8" t="s">
         <v>190</v>
-      </c>
-      <c r="K8" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
@@ -1919,16 +2137,16 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F9">
-        <v>6.7799999999999996E-3</v>
+        <v>330</v>
       </c>
       <c r="G9" t="s">
-        <v>195</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J9" t="s">
         <v>190</v>
@@ -1939,16 +2157,16 @@
         <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F10">
-        <v>330</v>
+        <v>126000</v>
       </c>
       <c r="G10" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="H10" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="J10" t="s">
         <v>190</v>
@@ -1959,36 +2177,36 @@
         <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F11">
-        <v>126000</v>
+        <v>20000</v>
       </c>
       <c r="G11" t="s">
         <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="J11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F12">
-        <v>20000</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="J12" t="s">
         <v>190</v>
@@ -1999,19 +2217,22 @@
         <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F13">
-        <v>20</v>
+        <v>500</v>
       </c>
       <c r="G13" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="H13" t="s">
         <v>206</v>
       </c>
       <c r="J13" t="s">
         <v>190</v>
+      </c>
+      <c r="K13" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2019,13 +2240,13 @@
         <v>181</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F14">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
         <v>206</v>
@@ -2033,42 +2254,16 @@
       <c r="J14" t="s">
         <v>190</v>
       </c>
-      <c r="K14" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" t="s">
-        <v>208</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" t="s">
-        <v>206</v>
-      </c>
-      <c r="J15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H16" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="J16" t="s">
         <v>209</v>
@@ -2079,10 +2274,10 @@
         <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s">
         <v>212</v>
@@ -2096,10 +2291,13 @@
         <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>212</v>
       </c>
       <c r="J18" t="s">
         <v>209</v>
@@ -2110,10 +2308,10 @@
         <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="J19" t="s">
         <v>209</v>
@@ -2124,7 +2322,7 @@
         <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G20" t="s">
         <v>88</v>
@@ -2138,19 +2336,13 @@
         <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" t="s">
-        <v>217</v>
+        <v>88</v>
       </c>
       <c r="J21" t="s">
         <v>209</v>
-      </c>
-      <c r="K21" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2158,10 +2350,13 @@
         <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G22" t="s">
         <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>217</v>
       </c>
       <c r="J22" t="s">
         <v>209</v>
@@ -2175,10 +2370,10 @@
         <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G23" t="s">
-        <v>121</v>
+        <v>26</v>
       </c>
       <c r="J23" t="s">
         <v>209</v>
@@ -2192,13 +2387,16 @@
         <v>181</v>
       </c>
       <c r="B24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="J24" t="s">
         <v>209</v>
+      </c>
+      <c r="K24" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2206,10 +2404,10 @@
         <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="J25" t="s">
         <v>209</v>
@@ -2220,13 +2418,10 @@
         <v>181</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="J26" t="s">
         <v>209</v>
@@ -2237,30 +2432,33 @@
         <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>224</v>
       </c>
       <c r="J27" t="s">
         <v>209</v>
       </c>
-      <c r="K27" t="s">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" t="s">
+        <v>223</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" t="s">
+        <v>209</v>
+      </c>
+      <c r="K28" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>181</v>
-      </c>
-      <c r="B30" t="s">
-        <v>225</v>
-      </c>
-      <c r="G30" t="s">
-        <v>121</v>
-      </c>
-      <c r="J30" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2268,7 +2466,7 @@
         <v>181</v>
       </c>
       <c r="B31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G31" t="s">
         <v>121</v>
@@ -2282,7 +2480,7 @@
         <v>181</v>
       </c>
       <c r="B32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G32" t="s">
         <v>121</v>
@@ -2296,10 +2494,10 @@
         <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="J33" t="s">
         <v>232</v>
@@ -2310,7 +2508,7 @@
         <v>181</v>
       </c>
       <c r="B34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G34" t="s">
         <v>26</v>
@@ -2324,10 +2522,10 @@
         <v>181</v>
       </c>
       <c r="B35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="J35" t="s">
         <v>232</v>
@@ -2338,12 +2536,26 @@
         <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G36" t="s">
         <v>88</v>
       </c>
       <c r="J36" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" t="s">
+        <v>231</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="J37" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2355,11 +2567,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,39 +2683,16 @@
         <v>233</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>88</v>
+      </c>
+      <c r="H7" t="s">
+        <v>235</v>
       </c>
       <c r="J7" t="s">
-        <v>190</v>
-      </c>
-      <c r="K7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>233</v>
-      </c>
-      <c r="B8" t="s">
-        <v>239</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2511,24 +2700,47 @@
         <v>233</v>
       </c>
       <c r="B9" t="s">
-        <v>242</v>
+        <v>237</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" t="s">
+        <v>190</v>
+      </c>
+      <c r="K9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>88</v>
       </c>
-      <c r="H9" t="s">
-        <v>235</v>
-      </c>
-      <c r="J9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
+      <c r="J10" t="s">
+        <v>190</v>
+      </c>
+      <c r="K10" t="s">
+        <v>238</v>
+      </c>
+    </row>
     <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2539,9 +2751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,7 +2969,7 @@
       <c r="C2" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>275</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -2774,7 +2986,7 @@
       <c r="C3" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>275</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -2839,10 +3051,10 @@
       <c r="B8" t="s">
         <v>262</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>2.7182818284590402</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>275</v>
       </c>
       <c r="J8" t="s">
@@ -2850,8 +3062,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="4"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2877,7 +3089,7 @@
       <c r="B11" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>275</v>
       </c>
       <c r="H11" t="s">
@@ -2958,7 +3170,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,10 +3296,10 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
       <c r="G9" t="s">
         <v>88</v>
       </c>
@@ -3102,7 +3314,7 @@
       <c r="C10" t="s">
         <v>289</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>275</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -3137,16 +3349,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3181,8 +3396,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -3195,8 +3410,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>292</v>
       </c>
@@ -3207,8 +3421,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>293</v>
       </c>
@@ -3219,8 +3432,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>294</v>
       </c>
@@ -3230,27 +3442,21 @@
       <c r="F5" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>275</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>185.13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -3258,13 +3464,13 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="7">
         <v>263.43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -3272,13 +3478,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>48</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>121</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -3286,16 +3492,16 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>21.13</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>327</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -3303,13 +3509,13 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>50</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="9" t="s">
@@ -3320,13 +3526,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>780</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>93</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -3334,13 +3540,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>71.061300000000003</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>329</v>
       </c>
       <c r="H13" s="9" t="s">
@@ -3351,13 +3557,13 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>56.033999999999999</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>329</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -3368,13 +3574,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>37.822949999999999</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>329</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -3385,13 +3591,13 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>71.061300000000003</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>329</v>
       </c>
       <c r="H16" s="9" t="s">
@@ -3402,13 +3608,13 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>28.3</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>332</v>
       </c>
       <c r="H17" s="9" t="s">
@@ -3419,13 +3625,13 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>28.3</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>333</v>
       </c>
       <c r="H18" s="9" t="s">
@@ -3436,13 +3642,13 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>137.53800000000001</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J19" s="2" t="s">
@@ -3450,13 +3656,13 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>48</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>121</v>
       </c>
       <c r="H20" s="9" t="s">
@@ -3467,14 +3673,14 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <f>20.376*2</f>
         <v>40.752000000000002</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>336</v>
       </c>
       <c r="H21" s="9"/>
@@ -3483,13 +3689,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>64.184399999999997</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J22" s="2" t="s">
@@ -3497,13 +3703,13 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>213.94800000000001</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="2" t="s">
         <v>335</v>
       </c>
       <c r="J23" s="2" t="s">
@@ -3511,13 +3717,13 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>144.6686</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -3525,13 +3731,13 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>132.44399999999999</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="2" t="s">
         <v>336</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -3539,13 +3745,13 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>24.4512</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -3553,13 +3759,13 @@
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>64.184399999999997</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -3567,13 +3773,13 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>156.89519999999999</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J28" s="2" t="s">
@@ -3581,13 +3787,13 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>42.7896</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -3595,13 +3801,13 @@
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>20.376000000000001</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -3609,16 +3815,16 @@
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>9.157</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="2" t="s">
         <v>334</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -3626,16 +3832,16 @@
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>3</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="4" t="s">
         <v>275</v>
       </c>
       <c r="J32" s="2" t="s">
@@ -3643,13 +3849,13 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>0</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -3657,77 +3863,77 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H37" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="2" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3739,20 +3945,23 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3787,48 +3996,744 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="J6" s="2"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="F8" s="4"/>
-      <c r="J8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G9" s="6"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="F10" s="2">
+        <v>780</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="14.45" x14ac:dyDescent="0.3"/>
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="F11" s="2">
+        <v>70.3</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8.3145100000000003</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="F13" s="2">
+        <v>26.5</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="F15" s="2">
+        <v>296</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F19" s="2">
+        <v>74</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F20" s="2">
+        <v>100</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F22" s="2">
+        <v>6.5700000000000003E-3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F23" s="2">
+        <v>13.1</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="F26" s="2">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F28" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="F29" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="F30" s="2">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed dependent variables from master table
</commit_message>
<xml_diff>
--- a/MSDO/MasterTable_rev1.xlsx
+++ b/MSDO/MasterTable_rev1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="466">
   <si>
     <t>Modules</t>
   </si>
@@ -1820,10 +1820,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:K288"/>
+  <dimension ref="A1:K266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B295" sqref="B295"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I226" sqref="I226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4696,13 +4696,13 @@
         <v>167</v>
       </c>
       <c r="B156" t="s">
-        <v>172</v>
+        <v>211</v>
       </c>
       <c r="G156" t="s">
-        <v>175</v>
+        <v>110</v>
       </c>
       <c r="J156" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
@@ -4710,16 +4710,13 @@
         <v>167</v>
       </c>
       <c r="B157" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="G157" t="s">
-        <v>78</v>
-      </c>
-      <c r="H157" t="s">
-        <v>198</v>
+        <v>110</v>
       </c>
       <c r="J157" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.3">
@@ -4727,16 +4724,13 @@
         <v>167</v>
       </c>
       <c r="B158" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="G158" t="s">
-        <v>26</v>
-      </c>
-      <c r="H158" t="s">
-        <v>198</v>
+        <v>110</v>
       </c>
       <c r="J158" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.3">
@@ -4744,13 +4738,13 @@
         <v>167</v>
       </c>
       <c r="B159" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="G159" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="J159" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
@@ -4758,13 +4752,13 @@
         <v>167</v>
       </c>
       <c r="B160" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="G160" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="J160" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.3">
@@ -4772,13 +4766,13 @@
         <v>167</v>
       </c>
       <c r="B161" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G161" t="s">
         <v>78</v>
       </c>
       <c r="J161" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.3">
@@ -4786,224 +4780,209 @@
         <v>167</v>
       </c>
       <c r="B162" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="G162" t="s">
-        <v>26</v>
-      </c>
-      <c r="H162" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="J162" t="s">
-        <v>195</v>
-      </c>
-      <c r="K162" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>167</v>
-      </c>
-      <c r="B163" t="s">
-        <v>204</v>
-      </c>
-      <c r="G163" t="s">
-        <v>26</v>
-      </c>
-      <c r="J163" t="s">
-        <v>195</v>
-      </c>
-      <c r="K163" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J163" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>167</v>
-      </c>
-      <c r="B164" t="s">
-        <v>205</v>
-      </c>
-      <c r="G164" t="s">
+        <v>219</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G164" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J164" t="s">
-        <v>195</v>
-      </c>
-      <c r="K164" t="s">
-        <v>186</v>
+      <c r="J164" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="B165" t="s">
-        <v>206</v>
+        <v>223</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
       </c>
       <c r="G165" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="J165" t="s">
-        <v>195</v>
+        <v>176</v>
+      </c>
+      <c r="K165" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="B166" t="s">
-        <v>207</v>
+        <v>225</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
       </c>
       <c r="G166" t="s">
         <v>78</v>
       </c>
       <c r="J166" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+      <c r="K166" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>167</v>
-      </c>
-      <c r="B167" t="s">
-        <v>208</v>
-      </c>
-      <c r="G167" t="s">
-        <v>110</v>
-      </c>
-      <c r="H167" t="s">
-        <v>210</v>
-      </c>
-      <c r="J167" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J167" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>167</v>
-      </c>
-      <c r="B168" t="s">
-        <v>209</v>
-      </c>
-      <c r="G168" t="s">
-        <v>78</v>
-      </c>
-      <c r="J168" t="s">
-        <v>195</v>
-      </c>
-      <c r="K168" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J168" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>167</v>
-      </c>
-      <c r="B169" t="s">
-        <v>211</v>
-      </c>
-      <c r="G169" t="s">
-        <v>110</v>
-      </c>
-      <c r="J169" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J169" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>167</v>
-      </c>
-      <c r="B170" t="s">
-        <v>212</v>
-      </c>
-      <c r="G170" t="s">
-        <v>110</v>
-      </c>
-      <c r="J170" t="s">
-        <v>218</v>
+        <v>1</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>167</v>
-      </c>
-      <c r="B171" t="s">
-        <v>213</v>
-      </c>
-      <c r="G171" t="s">
-        <v>110</v>
+        <v>1</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="J171" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>167</v>
-      </c>
-      <c r="B172" t="s">
-        <v>214</v>
-      </c>
-      <c r="G172" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="J172" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>167</v>
-      </c>
-      <c r="B173" t="s">
-        <v>215</v>
-      </c>
-      <c r="G173" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="J173" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>167</v>
-      </c>
-      <c r="B174" t="s">
-        <v>216</v>
-      </c>
-      <c r="G174" t="s">
-        <v>78</v>
-      </c>
-      <c r="J174" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J174" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>167</v>
-      </c>
-      <c r="B175" t="s">
-        <v>217</v>
-      </c>
-      <c r="G175" t="s">
-        <v>78</v>
-      </c>
-      <c r="J175" t="s">
-        <v>218</v>
+        <v>14</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>174</v>
+        <v>259</v>
       </c>
       <c r="J176" s="2" t="s">
         <v>173</v>
@@ -5011,13 +4990,16 @@
     </row>
     <row r="177" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>227</v>
+        <v>243</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="J177" s="2" t="s">
         <v>173</v>
@@ -5025,115 +5007,109 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B178" t="s">
-        <v>220</v>
+        <v>245</v>
+      </c>
+      <c r="C178" t="s">
+        <v>246</v>
+      </c>
+      <c r="F178">
+        <v>9.8665000000000003E-3</v>
       </c>
       <c r="G178" t="s">
-        <v>78</v>
-      </c>
-      <c r="H178" t="s">
-        <v>221</v>
+        <v>260</v>
       </c>
       <c r="J178" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B179" t="s">
-        <v>222</v>
-      </c>
-      <c r="G179" t="s">
-        <v>110</v>
-      </c>
-      <c r="H179" t="s">
-        <v>221</v>
+        <v>248</v>
+      </c>
+      <c r="F179" s="3">
+        <v>2.7182818284590402</v>
+      </c>
+      <c r="G179" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="J179" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B180" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="G180" t="s">
         <v>78</v>
       </c>
-      <c r="H180" t="s">
-        <v>221</v>
-      </c>
       <c r="J180" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B181" t="s">
-        <v>223</v>
-      </c>
-      <c r="F181">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="G181" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="J181" t="s">
-        <v>176</v>
-      </c>
-      <c r="K181" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="B182" t="s">
-        <v>225</v>
-      </c>
-      <c r="F182">
-        <v>0</v>
+        <v>256</v>
       </c>
       <c r="G182" t="s">
         <v>78</v>
       </c>
       <c r="J182" t="s">
-        <v>176</v>
-      </c>
-      <c r="K182" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="183" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="J183" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="K183" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="184" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>231</v>
+        <v>265</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="J184" s="2" t="s">
         <v>173</v>
@@ -5141,448 +5117,518 @@
     </row>
     <row r="185" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G185" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H185" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="J185" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>236</v>
+        <v>273</v>
+      </c>
+      <c r="G186" t="s">
+        <v>78</v>
       </c>
       <c r="J186" s="2" t="s">
-        <v>173</v>
+        <v>218</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B187" t="s">
-        <v>233</v>
-      </c>
-      <c r="C187" t="s">
-        <v>235</v>
+        <v>270</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="G187" t="s">
-        <v>259</v>
-      </c>
-      <c r="J187" t="s">
-        <v>195</v>
+        <v>78</v>
+      </c>
+      <c r="J187" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>1</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="J188" t="s">
-        <v>238</v>
+        <v>2</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F188" s="3"/>
+      <c r="G188" t="s">
+        <v>78</v>
+      </c>
+      <c r="J188" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>1</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J189" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
-        <v>1</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J190" t="s">
-        <v>238</v>
+        <v>2</v>
+      </c>
+      <c r="B189" t="s">
+        <v>272</v>
+      </c>
+      <c r="C189" t="s">
+        <v>275</v>
+      </c>
+      <c r="G189" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J189" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G190" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J190" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="191" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
-        <v>14</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="G191" s="4" t="s">
-        <v>261</v>
+      <c r="A191" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G191" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="J191" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="192" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
-        <v>14</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="G192" s="4" t="s">
-        <v>261</v>
+      <c r="A192" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="G192" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="J192" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="193" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
-        <v>14</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G193" s="2" t="s">
-        <v>259</v>
+    <row r="193" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="J193" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="194" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
-        <v>14</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>244</v>
+    <row r="194" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="F194" s="2">
+        <v>185.13</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="J194" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
-        <v>14</v>
-      </c>
-      <c r="B195" t="s">
-        <v>245</v>
-      </c>
-      <c r="C195" t="s">
-        <v>246</v>
-      </c>
-      <c r="F195">
-        <v>9.8665000000000003E-3</v>
-      </c>
-      <c r="G195" t="s">
-        <v>260</v>
-      </c>
-      <c r="J195" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>14</v>
-      </c>
-      <c r="B196" t="s">
-        <v>248</v>
-      </c>
-      <c r="F196" s="3">
-        <v>2.7182818284590402</v>
-      </c>
-      <c r="G196" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="J196" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
-        <v>14</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C197" t="s">
-        <v>250</v>
-      </c>
-      <c r="G197" t="s">
-        <v>78</v>
-      </c>
-      <c r="J197" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
-        <v>14</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G198" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="H198" t="s">
-        <v>252</v>
-      </c>
-      <c r="J198" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
-        <v>14</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G199" t="s">
-        <v>78</v>
-      </c>
-      <c r="J199" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>14</v>
-      </c>
-      <c r="B200" t="s">
-        <v>254</v>
-      </c>
-      <c r="G200" t="s">
-        <v>78</v>
-      </c>
-      <c r="J200" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>14</v>
-      </c>
-      <c r="B201" t="s">
-        <v>255</v>
-      </c>
-      <c r="G201" t="s">
-        <v>78</v>
-      </c>
-      <c r="J201" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>14</v>
-      </c>
-      <c r="B202" t="s">
-        <v>256</v>
-      </c>
-      <c r="G202" t="s">
-        <v>78</v>
-      </c>
-      <c r="J202" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="203" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
-        <v>2</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>263</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F195" s="7">
+        <v>263.43</v>
+      </c>
+      <c r="G195" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J195" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F196" s="2">
+        <v>48</v>
+      </c>
+      <c r="G196" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J196" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="F197" s="2">
+        <v>21.13</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="J197" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F198" s="2">
+        <v>50</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H198" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="J198" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F199" s="2">
+        <v>780</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J199" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F200" s="2">
+        <v>71.061300000000003</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H200" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J200" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F201" s="2">
+        <v>56.033999999999999</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H201" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J201" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F202" s="2">
+        <v>37.822949999999999</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H202" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J202" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A203" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="F203" s="2">
+        <v>71.061300000000003</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="H203" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="J203" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="K203" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="204" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
-        <v>2</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>266</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="F204" s="2">
+        <v>28.3</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="H204" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="J204" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="205" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
-        <v>2</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>267</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B205" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F205" s="2">
+        <v>28.3</v>
       </c>
       <c r="G205" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H205" s="2" t="s">
-        <v>268</v>
+        <v>319</v>
+      </c>
+      <c r="H205" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="J205" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
-        <v>2</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="G206" t="s">
-        <v>78</v>
+    <row r="206" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="F206" s="2">
+        <v>137.53800000000001</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="J206" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
-        <v>2</v>
-      </c>
-      <c r="B207" t="s">
-        <v>270</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="G207" t="s">
-        <v>78</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="F207" s="2">
+        <v>48</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H207" s="9" t="s">
+        <v>320</v>
       </c>
       <c r="J207" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
-        <v>2</v>
-      </c>
-      <c r="B208" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="F208" s="3"/>
-      <c r="G208" t="s">
-        <v>78</v>
-      </c>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F208" s="2">
+        <v>40.752000000000002</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H208" s="9"/>
       <c r="J208" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
-        <v>2</v>
-      </c>
-      <c r="B209" t="s">
-        <v>272</v>
-      </c>
-      <c r="C209" t="s">
-        <v>275</v>
-      </c>
-      <c r="G209" s="5" t="s">
-        <v>261</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B209" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F209" s="2">
+        <v>64.184399999999997</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="J209" s="2" t="s">
-        <v>218</v>
+        <v>176</v>
       </c>
     </row>
     <row r="210" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B210" s="8" t="s">
-        <v>277</v>
+      <c r="B210" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F210" s="2">
+        <v>213.94800000000001</v>
       </c>
       <c r="G210" s="2" t="s">
-        <v>174</v>
+        <v>321</v>
       </c>
       <c r="J210" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="211" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B211" s="8" t="s">
-        <v>278</v>
+      <c r="B211" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F211" s="2">
+        <v>144.6686</v>
       </c>
       <c r="G211" s="2" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="J211" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="212" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B212" s="8" t="s">
-        <v>279</v>
+      <c r="B212" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F212" s="2">
+        <v>132.44399999999999</v>
       </c>
       <c r="G212" s="2" t="s">
-        <v>124</v>
+        <v>322</v>
       </c>
       <c r="J212" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="213" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B213" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C213" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F213" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="G213" s="4" t="s">
-        <v>261</v>
+      <c r="B213" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F213" s="2">
+        <v>24.4512</v>
+      </c>
+      <c r="G213" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="J213" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="214" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5590,10 +5636,10 @@
         <v>3</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="F214" s="2">
-        <v>185.13</v>
+        <v>64.184399999999997</v>
       </c>
       <c r="G214" s="2" t="s">
         <v>110</v>
@@ -5607,10 +5653,10 @@
         <v>3</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="F215" s="7">
-        <v>263.43</v>
+        <v>306</v>
+      </c>
+      <c r="F215" s="2">
+        <v>156.89519999999999</v>
       </c>
       <c r="G215" s="2" t="s">
         <v>110</v>
@@ -5624,12 +5670,12 @@
         <v>3</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="F216" s="2">
-        <v>48</v>
-      </c>
-      <c r="G216" s="4" t="s">
+        <v>42.7896</v>
+      </c>
+      <c r="G216" s="2" t="s">
         <v>110</v>
       </c>
       <c r="J216" s="2" t="s">
@@ -5641,16 +5687,13 @@
         <v>3</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="F217" s="2">
-        <v>21.13</v>
+        <v>20.376000000000001</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="H217" s="2" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="J217" s="2" t="s">
         <v>176</v>
@@ -5661,16 +5704,16 @@
         <v>3</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="F218" s="2">
-        <v>50</v>
+        <v>9.157</v>
       </c>
       <c r="G218" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H218" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
+      </c>
+      <c r="H218" s="2" t="s">
+        <v>320</v>
       </c>
       <c r="J218" s="2" t="s">
         <v>176</v>
@@ -5681,13 +5724,16 @@
         <v>3</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>288</v>
+        <v>310</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="F219" s="2">
-        <v>780</v>
-      </c>
-      <c r="G219" s="2" t="s">
-        <v>83</v>
+        <v>3</v>
+      </c>
+      <c r="G219" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="J219" s="2" t="s">
         <v>176</v>
@@ -5698,16 +5744,13 @@
         <v>3</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>289</v>
+        <v>311</v>
       </c>
       <c r="F220" s="2">
-        <v>71.061300000000003</v>
+        <v>0</v>
       </c>
       <c r="G220" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H220" s="9" t="s">
-        <v>316</v>
+        <v>26</v>
       </c>
       <c r="J220" s="2" t="s">
         <v>176</v>
@@ -5718,19 +5761,13 @@
         <v>3</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="F221" s="2">
-        <v>56.033999999999999</v>
+        <v>324</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H221" s="9" t="s">
-        <v>316</v>
+        <v>110</v>
       </c>
       <c r="J221" s="2" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="222" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5738,19 +5775,13 @@
         <v>3</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="F222" s="2">
-        <v>37.822949999999999</v>
+        <v>325</v>
       </c>
       <c r="G222" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H222" s="9" t="s">
-        <v>316</v>
+        <v>78</v>
       </c>
       <c r="J222" s="2" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="223" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5758,19 +5789,13 @@
         <v>3</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="F223" s="2">
-        <v>71.061300000000003</v>
+        <v>326</v>
       </c>
       <c r="G223" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="H223" s="9" t="s">
-        <v>316</v>
+        <v>26</v>
       </c>
       <c r="J223" s="2" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="224" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -5778,394 +5803,420 @@
         <v>3</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="F224" s="2">
-        <v>28.3</v>
+        <v>327</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="H224" s="9" t="s">
-        <v>316</v>
+        <v>78</v>
       </c>
       <c r="J224" s="2" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="225" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F225" s="2">
-        <v>28.3</v>
+        <v>329</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="H225" s="9" t="s">
-        <v>316</v>
+        <v>110</v>
       </c>
       <c r="J225" s="2" t="s">
-        <v>176</v>
+        <v>337</v>
       </c>
     </row>
     <row r="226" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="F226" s="2">
-        <v>137.53800000000001</v>
+        <v>330</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="J226" s="2" t="s">
-        <v>176</v>
+        <v>337</v>
       </c>
     </row>
     <row r="227" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B227" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="F227" s="2">
-        <v>48</v>
+        <v>4</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H227" s="9" t="s">
-        <v>320</v>
+        <v>174</v>
       </c>
       <c r="J227" s="2" t="s">
-        <v>176</v>
+        <v>337</v>
       </c>
     </row>
     <row r="228" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="F228" s="2">
-        <v>40.752000000000002</v>
+        <v>278</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="H228" s="9"/>
+        <v>32</v>
+      </c>
       <c r="J228" s="2" t="s">
-        <v>176</v>
+        <v>337</v>
       </c>
     </row>
     <row r="229" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>300</v>
+        <v>331</v>
       </c>
       <c r="F229" s="2">
-        <v>64.184399999999997</v>
+        <v>2</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>110</v>
+        <v>334</v>
       </c>
       <c r="J229" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="230" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>301</v>
+        <v>332</v>
       </c>
       <c r="F230" s="2">
-        <v>213.94800000000001</v>
+        <v>4</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="J230" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="231" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="F231" s="2">
-        <v>144.6686</v>
+        <v>333</v>
+      </c>
+      <c r="F231" s="7">
+        <v>6</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>110</v>
+        <v>336</v>
       </c>
       <c r="J231" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="232" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>303</v>
+        <v>339</v>
       </c>
       <c r="F232" s="2">
-        <v>132.44399999999999</v>
-      </c>
-      <c r="G232" s="2" t="s">
-        <v>322</v>
+        <v>780</v>
+      </c>
+      <c r="G232" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="J232" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="233" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="F233" s="2">
-        <v>24.4512</v>
+        <v>70.3</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>110</v>
+        <v>363</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>364</v>
       </c>
       <c r="J233" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="234" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
       <c r="F234" s="2">
-        <v>64.184399999999997</v>
+        <v>8.3145100000000003</v>
       </c>
       <c r="G234" s="2" t="s">
-        <v>110</v>
+        <v>365</v>
       </c>
       <c r="J234" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="235" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>306</v>
+        <v>342</v>
       </c>
       <c r="F235" s="2">
-        <v>156.89519999999999</v>
+        <v>26.5</v>
       </c>
       <c r="G235" s="2" t="s">
-        <v>110</v>
+        <v>32</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="J235" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="236" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>307</v>
+        <v>343</v>
       </c>
       <c r="F236" s="2">
-        <v>42.7896</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="G236" s="2" t="s">
-        <v>110</v>
+        <v>32</v>
+      </c>
+      <c r="H236" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="J236" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="237" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>308</v>
+        <v>344</v>
       </c>
       <c r="F237" s="2">
-        <v>20.376000000000001</v>
+        <v>296</v>
       </c>
       <c r="G237" s="2" t="s">
-        <v>110</v>
+        <v>367</v>
+      </c>
+      <c r="H237" s="2" t="s">
+        <v>366</v>
       </c>
       <c r="J237" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="238" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>309</v>
+        <v>345</v>
       </c>
       <c r="F238" s="2">
-        <v>9.157</v>
+        <v>0.05</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>312</v>
+        <v>368</v>
       </c>
       <c r="H238" s="2" t="s">
-        <v>320</v>
+        <v>366</v>
       </c>
       <c r="J238" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="239" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>323</v>
+        <v>346</v>
       </c>
       <c r="F239" s="2">
-        <v>3</v>
-      </c>
-      <c r="G239" s="4" t="s">
-        <v>261</v>
+        <v>1.04</v>
+      </c>
+      <c r="G239" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="J239" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="240" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>311</v>
+        <v>347</v>
       </c>
       <c r="F240" s="2">
-        <v>0</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="G240" s="2" t="s">
-        <v>26</v>
+        <v>369</v>
+      </c>
+      <c r="H240" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="J240" s="2" t="s">
-        <v>176</v>
+        <v>338</v>
       </c>
     </row>
     <row r="241" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>293</v>
+        <v>348</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F241" s="2">
+        <v>74</v>
       </c>
       <c r="G241" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H241" s="2" t="s">
-        <v>317</v>
+        <v>32</v>
       </c>
       <c r="J241" s="2" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
     </row>
     <row r="242" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>297</v>
+        <v>349</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F242" s="2">
+        <v>100</v>
       </c>
       <c r="G242" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H242" s="2" t="s">
-        <v>317</v>
+        <v>32</v>
       </c>
       <c r="J242" s="2" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
     </row>
     <row r="243" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>324</v>
+        <v>350</v>
+      </c>
+      <c r="F243" s="2">
+        <v>2.2999999999999998</v>
       </c>
       <c r="G243" s="2" t="s">
-        <v>110</v>
+        <v>369</v>
+      </c>
+      <c r="H243" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="J243" s="2" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
     </row>
     <row r="244" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>325</v>
+        <v>351</v>
+      </c>
+      <c r="F244" s="2">
+        <v>6.5700000000000003E-3</v>
       </c>
       <c r="G244" s="2" t="s">
-        <v>78</v>
+        <v>110</v>
+      </c>
+      <c r="H244" s="2" t="s">
+        <v>373</v>
       </c>
       <c r="J244" s="2" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
     </row>
     <row r="245" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>326</v>
+        <v>353</v>
+      </c>
+      <c r="F245" s="2">
+        <v>13.1</v>
       </c>
       <c r="G245" s="2" t="s">
-        <v>26</v>
+        <v>374</v>
+      </c>
+      <c r="H245" s="2" t="s">
+        <v>375</v>
       </c>
       <c r="J245" s="2" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
     </row>
     <row r="246" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>327</v>
+        <v>354</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F246" s="2">
+        <v>0.83</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>78</v>
+        <v>376</v>
+      </c>
+      <c r="H246" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="J246" s="2" t="s">
-        <v>218</v>
+        <v>338</v>
       </c>
     </row>
     <row r="247" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6173,13 +6224,22 @@
         <v>4</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>329</v>
+        <v>355</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F247" s="2">
+        <v>0.17</v>
       </c>
       <c r="G247" s="2" t="s">
-        <v>110</v>
+        <v>376</v>
+      </c>
+      <c r="H247" s="2" t="s">
+        <v>377</v>
       </c>
       <c r="J247" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="248" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6187,27 +6247,39 @@
         <v>4</v>
       </c>
       <c r="B248" s="7" t="s">
-        <v>330</v>
+        <v>356</v>
+      </c>
+      <c r="F248" s="2">
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="G248" s="2" t="s">
-        <v>78</v>
+        <v>380</v>
+      </c>
+      <c r="H248" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="J248" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="249" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B249" s="8" t="s">
-        <v>277</v>
+      <c r="B249" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F249" s="2">
+        <v>2.9</v>
       </c>
       <c r="G249" s="2" t="s">
-        <v>174</v>
+        <v>110</v>
+      </c>
+      <c r="H249" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="J249" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="250" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6215,16 +6287,19 @@
         <v>4</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C250" s="2" t="s">
-        <v>352</v>
+        <v>358</v>
+      </c>
+      <c r="F250" s="2">
+        <v>13.8</v>
       </c>
       <c r="G250" s="2" t="s">
-        <v>32</v>
+        <v>363</v>
+      </c>
+      <c r="H250" s="2" t="s">
+        <v>384</v>
       </c>
       <c r="J250" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="251" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -6232,13 +6307,16 @@
         <v>4</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>331</v>
+        <v>359</v>
       </c>
       <c r="F251" s="2">
-        <v>2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G251" s="2" t="s">
-        <v>334</v>
+        <v>380</v>
+      </c>
+      <c r="H251" s="2" t="s">
+        <v>385</v>
       </c>
       <c r="J251" s="2" t="s">
         <v>338</v>
@@ -6249,13 +6327,16 @@
         <v>4</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="F252" s="2">
-        <v>4</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="G252" s="2" t="s">
-        <v>335</v>
+        <v>380</v>
+      </c>
+      <c r="H252" s="2" t="s">
+        <v>382</v>
       </c>
       <c r="J252" s="2" t="s">
         <v>338</v>
@@ -6266,13 +6347,16 @@
         <v>4</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="F253" s="7">
-        <v>6</v>
+        <v>361</v>
+      </c>
+      <c r="F253" s="2">
+        <v>0.625</v>
       </c>
       <c r="G253" s="2" t="s">
-        <v>336</v>
+        <v>369</v>
+      </c>
+      <c r="H253" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="J253" s="2" t="s">
         <v>338</v>
@@ -6283,13 +6367,16 @@
         <v>4</v>
       </c>
       <c r="B254" s="7" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="F254" s="2">
-        <v>780</v>
-      </c>
-      <c r="G254" s="4" t="s">
-        <v>83</v>
+        <v>0.24</v>
+      </c>
+      <c r="G254" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H254" s="2" t="s">
+        <v>385</v>
       </c>
       <c r="J254" s="2" t="s">
         <v>338</v>
@@ -6299,610 +6386,167 @@
       <c r="A255" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B255" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="F255" s="2">
-        <v>70.3</v>
+      <c r="B255" s="8" t="s">
+        <v>387</v>
       </c>
       <c r="G255" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H255" s="2" t="s">
-        <v>364</v>
+        <v>78</v>
       </c>
       <c r="J255" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="256" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B256" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="F256" s="2">
-        <v>8.3145100000000003</v>
+      <c r="B256" s="8" t="s">
+        <v>388</v>
       </c>
       <c r="G256" s="2" t="s">
-        <v>365</v>
+        <v>110</v>
       </c>
       <c r="J256" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="257" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B257" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="F257" s="2">
-        <v>26.5</v>
+      <c r="B257" s="8" t="s">
+        <v>389</v>
       </c>
       <c r="G257" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H257" s="2" t="s">
-        <v>366</v>
+        <v>78</v>
       </c>
       <c r="J257" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="258" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B258" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="F258" s="2">
-        <v>0.56999999999999995</v>
+      <c r="B258" s="8" t="s">
+        <v>390</v>
       </c>
       <c r="G258" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H258" s="2" t="s">
-        <v>366</v>
+        <v>110</v>
       </c>
       <c r="J258" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="259" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B259" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="F259" s="2">
-        <v>296</v>
+      <c r="B259" s="8" t="s">
+        <v>391</v>
       </c>
       <c r="G259" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="H259" s="2" t="s">
-        <v>366</v>
+        <v>78</v>
       </c>
       <c r="J259" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="260" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B260" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="F260" s="2">
-        <v>0.05</v>
+      <c r="B260" s="8" t="s">
+        <v>392</v>
       </c>
       <c r="G260" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="H260" s="2" t="s">
-        <v>366</v>
+        <v>26</v>
       </c>
       <c r="J260" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="261" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B261" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="F261" s="2">
-        <v>1.04</v>
+      <c r="B261" s="8" t="s">
+        <v>393</v>
       </c>
       <c r="G261" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H261" s="2" t="s">
-        <v>370</v>
+        <v>110</v>
       </c>
       <c r="J261" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="262" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B262" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="F262" s="2">
-        <v>0.81599999999999995</v>
+      <c r="B262" s="8" t="s">
+        <v>394</v>
       </c>
       <c r="G262" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H262" s="2" t="s">
-        <v>370</v>
+        <v>78</v>
       </c>
       <c r="J262" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="263" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B263" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F263" s="2">
-        <v>74</v>
+      <c r="B263" s="8" t="s">
+        <v>395</v>
       </c>
       <c r="G263" s="2" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="J263" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="264" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B264" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="C264" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F264" s="2">
-        <v>100</v>
+      <c r="B264" s="8" t="s">
+        <v>396</v>
       </c>
       <c r="G264" s="2" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="J264" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="265" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B265" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="F265" s="2">
-        <v>2.2999999999999998</v>
+      <c r="B265" s="8" t="s">
+        <v>397</v>
       </c>
       <c r="G265" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H265" s="2" t="s">
-        <v>373</v>
+        <v>110</v>
       </c>
       <c r="J265" s="2" t="s">
-        <v>338</v>
+        <v>238</v>
       </c>
     </row>
     <row r="266" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B266" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="F266" s="2">
-        <v>6.5700000000000003E-3</v>
+      <c r="B266" s="8" t="s">
+        <v>398</v>
       </c>
       <c r="G266" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H266" s="2" t="s">
-        <v>373</v>
+        <v>26</v>
       </c>
       <c r="J266" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="267" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B267" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="F267" s="2">
-        <v>13.1</v>
-      </c>
-      <c r="G267" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="H267" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="J267" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="268" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B268" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F268" s="2">
-        <v>0.83</v>
-      </c>
-      <c r="G268" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="H268" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="J268" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="269" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A269" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B269" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F269" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="G269" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="H269" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="J269" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="270" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B270" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="F270" s="2">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="G270" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H270" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="J270" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="271" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B271" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="F271" s="2">
-        <v>2.9</v>
-      </c>
-      <c r="G271" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H271" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="J271" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="272" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B272" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="F272" s="2">
-        <v>13.8</v>
-      </c>
-      <c r="G272" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H272" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="J272" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="273" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B273" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="F273" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G273" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H273" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J273" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="274" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B274" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="F274" s="2">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G274" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="H274" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="J274" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="275" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B275" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="F275" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="G275" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H275" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="J275" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="276" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B276" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="F276" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="G276" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H276" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J276" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="277" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A277" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B277" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="G277" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J277" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B278" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="G278" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J278" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B279" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="G279" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J279" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="280" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A280" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B280" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="G280" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J280" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A281" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B281" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="G281" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J281" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B282" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="G282" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J282" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="283" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B283" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="G283" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J283" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="284" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B284" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="G284" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J284" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="285" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B285" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="G285" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J285" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="286" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B286" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="G286" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J286" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="287" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B287" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="G287" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J287" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B288" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="G288" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J288" s="2" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>